<commit_message>
Datos CFD en perdida y casos de mandos aleron y rudder
</commit_message>
<xml_diff>
--- a/Modelo CFD DroneBoX/Hoja de casos CFD.xlsx
+++ b/Modelo CFD DroneBoX/Hoja de casos CFD.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
   <si>
     <t>Paquete</t>
   </si>
@@ -76,19 +76,13 @@
     <t>dbx_v1_s50_r16_a35_bX_da0_de0_dr0</t>
   </si>
   <si>
-    <t>dbx_v1_s50_r16_a50_bX_da0_de0_dr0</t>
-  </si>
-  <si>
-    <t>dbx_v1_s50_r16_am6_bX_da0_de0_dr0</t>
-  </si>
-  <si>
-    <t>dbx_v1_s50_r16_am18_bX_da0_de0_dr0</t>
-  </si>
-  <si>
-    <t>dbx_v1_s50_r16_am25_bX_da0_de0_dr0</t>
-  </si>
-  <si>
-    <t>Terminado</t>
+    <t>dbx_v1_s50_r16_a22_bX_da0_de0_dr0</t>
+  </si>
+  <si>
+    <t>dbx_v1_s50_r16_a30_bX_da0_de0_dr0</t>
+  </si>
+  <si>
+    <t>dbx_v1_s50_r16_a25_b0_da0_deX_dr0</t>
   </si>
 </sst>
 </file>
@@ -187,7 +181,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -195,14 +189,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -510,14 +507,14 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.5703125" style="7" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="32.42578125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="40.5703125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="32.42578125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -527,221 +524,183 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="3"/>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="C11" s="2"/>
+      <c r="J11" s="6"/>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="2" t="s">
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="C15" s="3"/>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="2"/>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="3"/>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="4"/>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J11" s="8"/>
-    </row>
-    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" s="3"/>
-    </row>
-    <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19" s="4"/>
-    </row>
-    <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>3</v>
-      </c>
       <c r="C20" s="4"/>
     </row>
     <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
       <c r="C21" s="4"/>
     </row>
   </sheetData>

</xml_diff>